<commit_message>
New batch of profiles (mainly rohan + mordor)
</commit_message>
<xml_diff>
--- a/src/mesbg_models.xlsx
+++ b/src/mesbg_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706B25E7-100A-442D-9532-AA927FBA41FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65AE9B9-E1C2-46C7-81BC-EE75A6F8BFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="192">
   <si>
     <t>faction</t>
   </si>
@@ -540,6 +540,81 @@
   </si>
   <si>
     <t>The Golden King</t>
+  </si>
+  <si>
+    <t>Aldor</t>
+  </si>
+  <si>
+    <t>Boromir of Gondor</t>
+  </si>
+  <si>
+    <t>Captain of Rohan</t>
+  </si>
+  <si>
+    <t>Deorwine</t>
+  </si>
+  <si>
+    <t>Elfhelm</t>
+  </si>
+  <si>
+    <t>Eorl the Young</t>
+  </si>
+  <si>
+    <t>Erkenbrand</t>
+  </si>
+  <si>
+    <t>Frodo Baggins</t>
+  </si>
+  <si>
+    <t>Gandalf the Grey</t>
+  </si>
+  <si>
+    <t>Gondor Battlecry Trebuchet</t>
+  </si>
+  <si>
+    <t>Grimbold</t>
+  </si>
+  <si>
+    <t>Haleth</t>
+  </si>
+  <si>
+    <t>Helm Hammerhand</t>
+  </si>
+  <si>
+    <t>Irolas</t>
+  </si>
+  <si>
+    <t>King of Men</t>
+  </si>
+  <si>
+    <t>King's Huntsman</t>
+  </si>
+  <si>
+    <t>Meriadoc Brandybuck</t>
+  </si>
+  <si>
+    <t>Mouth of Sauron</t>
+  </si>
+  <si>
+    <t>Peregrin Took</t>
+  </si>
+  <si>
+    <t>Rohan Outrider</t>
+  </si>
+  <si>
+    <t>Samwise Gamgee</t>
+  </si>
+  <si>
+    <t>Son of Eorl</t>
+  </si>
+  <si>
+    <t>The Dwimmerlaik</t>
+  </si>
+  <si>
+    <t>The Tainted</t>
+  </si>
+  <si>
+    <t>Theodred</t>
   </si>
 </sst>
 </file>
@@ -935,24 +1010,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
-  <dimension ref="A1:F142"/>
+  <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G159" sqref="G159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,18 +1047,18 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -992,18 +1067,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1012,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1052,18 +1127,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -1072,18 +1147,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>160</v>
+        <v>75</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1092,18 +1167,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1112,12 +1187,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -1132,18 +1207,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1152,18 +1227,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>75</v>
+        <v>160</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1172,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1192,32 +1267,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -1232,18 +1307,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1252,18 +1327,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1272,18 +1347,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1292,38 +1367,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
         <v>25</v>
       </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18">
-        <v>60</v>
-      </c>
       <c r="E18" t="b">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D19">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1332,18 +1407,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D20">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1352,18 +1427,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D21">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1372,18 +1447,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D22">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1392,18 +1467,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D23">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1412,18 +1487,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D24">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1432,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1452,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1472,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1492,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1512,7 +1587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1532,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1552,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1572,18 +1647,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1592,18 +1667,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D33">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1612,18 +1687,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
       </c>
       <c r="D34">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1632,18 +1707,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1652,12 +1727,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
@@ -1672,18 +1747,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D37">
-        <v>55</v>
+        <v>180</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1692,18 +1767,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D38">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1712,18 +1787,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D39">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1732,18 +1807,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
         <v>49</v>
       </c>
       <c r="D40">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1752,18 +1827,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D41">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1772,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1792,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -1812,7 +1887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1832,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1852,18 +1927,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D46">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1872,18 +1947,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D47">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1892,18 +1967,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>63</v>
       </c>
       <c r="B48" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
         <v>11</v>
       </c>
       <c r="D48">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1912,18 +1987,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
         <v>11</v>
       </c>
       <c r="D49">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1932,18 +2007,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C50" t="s">
         <v>11</v>
       </c>
       <c r="D50">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1952,18 +2027,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D51">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -1972,18 +2047,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D52">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -1992,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>63</v>
       </c>
@@ -2012,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -2032,7 +2107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -2052,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -2072,7 +2147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2092,18 +2167,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D58">
-        <v>225</v>
+        <v>50</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
@@ -2112,18 +2187,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C59" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D59">
-        <v>160</v>
+        <v>55</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -2132,18 +2207,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C60" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D60">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -2152,18 +2227,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D61">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -2172,18 +2247,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D62">
-        <v>220</v>
+        <v>55</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -2192,18 +2267,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D63">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -2212,18 +2287,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>181</v>
       </c>
       <c r="C64" t="s">
         <v>11</v>
       </c>
       <c r="D64">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -2232,18 +2307,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D65">
-        <v>55</v>
+        <v>225</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -2252,18 +2327,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D66">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -2272,18 +2347,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D67">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -2292,18 +2367,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D68">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
@@ -2312,18 +2387,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C69" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D69">
-        <v>35</v>
+        <v>220</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -2332,19 +2407,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
       <c r="B70" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70">
         <v>80</v>
       </c>
-      <c r="C70" t="s">
-        <v>24</v>
-      </c>
-      <c r="D70">
-        <v>30</v>
-      </c>
       <c r="E70" t="b">
         <v>0</v>
       </c>
@@ -2352,15 +2427,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C71" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D71">
         <v>25</v>
@@ -2372,12 +2447,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="C72" t="s">
         <v>24</v>
@@ -2392,18 +2467,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D73">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
@@ -2412,18 +2487,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C74" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D74">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
@@ -2432,18 +2507,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C75" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D75">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E75" t="b">
         <v>0</v>
@@ -2452,78 +2527,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C76" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D76">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
       </c>
       <c r="F76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>96</v>
+        <v>176</v>
       </c>
       <c r="C77" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D77">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="E77" t="b">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C78" t="s">
         <v>13</v>
       </c>
       <c r="D78">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C79" t="s">
         <v>13</v>
       </c>
       <c r="D79">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
@@ -2532,99 +2607,99 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="C80" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D80">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
       </c>
       <c r="F80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>76</v>
+      </c>
+      <c r="B81" t="s">
+        <v>96</v>
+      </c>
+      <c r="C81" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81">
+        <v>8</v>
+      </c>
+      <c r="E81" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" t="s">
+        <v>98</v>
+      </c>
+      <c r="C82" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82">
+        <v>8</v>
+      </c>
+      <c r="E82" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>76</v>
+      </c>
+      <c r="B83" t="s">
+        <v>99</v>
+      </c>
+      <c r="C83" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83">
+        <v>7</v>
+      </c>
+      <c r="E83" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>100</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B84" t="s">
         <v>101</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C84" t="s">
         <v>17</v>
       </c>
-      <c r="D81">
+      <c r="D84">
         <v>100</v>
       </c>
-      <c r="E81" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>102</v>
-      </c>
-      <c r="B82" t="s">
-        <v>123</v>
-      </c>
-      <c r="C82" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82">
-        <v>400</v>
-      </c>
-      <c r="E82" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>102</v>
-      </c>
-      <c r="B83" t="s">
-        <v>131</v>
-      </c>
-      <c r="C83" t="s">
-        <v>17</v>
-      </c>
-      <c r="D83">
-        <v>70</v>
-      </c>
-      <c r="E83" t="b">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>102</v>
-      </c>
-      <c r="B84" t="s">
-        <v>108</v>
-      </c>
-      <c r="C84" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84">
-        <v>130</v>
-      </c>
       <c r="E84" t="b">
         <v>0</v>
       </c>
@@ -2632,18 +2707,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>102</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D85">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="E85" t="b">
         <v>0</v>
@@ -2652,18 +2727,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>102</v>
       </c>
       <c r="B86" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D86">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="E86" t="b">
         <v>0</v>
@@ -2672,18 +2747,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>102</v>
       </c>
       <c r="B87" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D87">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E87" t="b">
         <v>0</v>
@@ -2692,18 +2767,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>102</v>
       </c>
       <c r="B88" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C88" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D88">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="E88" t="b">
         <v>0</v>
@@ -2712,18 +2787,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>102</v>
       </c>
       <c r="B89" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="C89" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D89">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E89" t="b">
         <v>0</v>
@@ -2732,18 +2807,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C90" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D90">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E90" t="b">
         <v>0</v>
@@ -2752,18 +2827,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
       </c>
       <c r="D91">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E91" t="b">
         <v>0</v>
@@ -2772,18 +2847,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C92" t="s">
         <v>11</v>
       </c>
       <c r="D92">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="E92" t="b">
         <v>0</v>
@@ -2792,12 +2867,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C93" t="s">
         <v>11</v>
@@ -2812,18 +2887,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>102</v>
       </c>
       <c r="B94" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="C94" t="s">
         <v>11</v>
       </c>
       <c r="D94">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E94" t="b">
         <v>0</v>
@@ -2832,18 +2907,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>102</v>
       </c>
       <c r="B95" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="C95" t="s">
         <v>11</v>
       </c>
       <c r="D95">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -2852,18 +2927,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D96">
-        <v>60</v>
+        <v>400</v>
       </c>
       <c r="E96" t="b">
         <v>0</v>
@@ -2872,18 +2947,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>102</v>
       </c>
       <c r="B97" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="C97" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D97">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E97" t="b">
         <v>0</v>
@@ -2892,18 +2967,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D98">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E98" t="b">
         <v>0</v>
@@ -2912,18 +2987,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>102</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C99" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D99">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
@@ -2932,18 +3007,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D100">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E100" t="b">
         <v>0</v>
@@ -2952,18 +3027,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C101" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D101">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E101" t="b">
         <v>0</v>
@@ -2972,18 +3047,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C102" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D102">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
@@ -2992,19 +3067,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
       <c r="B103" t="s">
+        <v>128</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103">
         <v>120</v>
       </c>
-      <c r="C103" t="s">
-        <v>49</v>
-      </c>
-      <c r="D103">
-        <v>30</v>
-      </c>
       <c r="E103" t="b">
         <v>0</v>
       </c>
@@ -3012,18 +3087,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="C104" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D104">
-        <v>9</v>
+        <v>120</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -3032,18 +3107,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>113</v>
+        <v>184</v>
       </c>
       <c r="C105" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D105">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -3052,18 +3127,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>189</v>
       </c>
       <c r="C106" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D106">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E106" t="b">
         <v>0</v>
@@ -3072,18 +3147,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>117</v>
+        <v>190</v>
       </c>
       <c r="C107" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D107">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="E107" t="b">
         <v>0</v>
@@ -3092,18 +3167,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>102</v>
       </c>
       <c r="B108" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C108" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D108">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E108" t="b">
         <v>0</v>
@@ -3112,18 +3187,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>102</v>
       </c>
       <c r="B109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C109" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D109">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
@@ -3132,18 +3207,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>102</v>
       </c>
       <c r="B110" t="s">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="C110" t="s">
         <v>13</v>
       </c>
       <c r="D110">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E110" t="b">
         <v>0</v>
@@ -3152,139 +3227,139 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>102</v>
       </c>
       <c r="B111" t="s">
+        <v>113</v>
+      </c>
+      <c r="C111" t="s">
+        <v>13</v>
+      </c>
+      <c r="D111">
+        <v>7</v>
+      </c>
+      <c r="E111" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>102</v>
+      </c>
+      <c r="B112" t="s">
+        <v>115</v>
+      </c>
+      <c r="C112" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112">
+        <v>100</v>
+      </c>
+      <c r="E112" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>102</v>
+      </c>
+      <c r="B113" t="s">
+        <v>117</v>
+      </c>
+      <c r="C113" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113">
+        <v>8</v>
+      </c>
+      <c r="E113" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>102</v>
+      </c>
+      <c r="B114" t="s">
+        <v>118</v>
+      </c>
+      <c r="C114" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114">
+        <v>18</v>
+      </c>
+      <c r="E114" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>102</v>
+      </c>
+      <c r="B115" t="s">
+        <v>122</v>
+      </c>
+      <c r="C115" t="s">
+        <v>13</v>
+      </c>
+      <c r="D115">
+        <v>5</v>
+      </c>
+      <c r="E115" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>102</v>
+      </c>
+      <c r="B116" t="s">
+        <v>130</v>
+      </c>
+      <c r="C116" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116">
+        <v>11</v>
+      </c>
+      <c r="E116" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>102</v>
+      </c>
+      <c r="B117" t="s">
         <v>103</v>
       </c>
-      <c r="C111" t="s">
-        <v>13</v>
-      </c>
-      <c r="D111">
+      <c r="C117" t="s">
+        <v>13</v>
+      </c>
+      <c r="D117">
         <v>12</v>
       </c>
-      <c r="E111" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>132</v>
-      </c>
-      <c r="B112" t="s">
-        <v>135</v>
-      </c>
-      <c r="C112" t="s">
-        <v>17</v>
-      </c>
-      <c r="D112">
-        <v>170</v>
-      </c>
-      <c r="E112" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>132</v>
-      </c>
-      <c r="B113" t="s">
-        <v>137</v>
-      </c>
-      <c r="C113" t="s">
-        <v>7</v>
-      </c>
-      <c r="D113">
-        <v>145</v>
-      </c>
-      <c r="E113" t="b">
-        <v>0</v>
-      </c>
-      <c r="F113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>132</v>
-      </c>
-      <c r="B114" t="s">
-        <v>133</v>
-      </c>
-      <c r="C114" t="s">
-        <v>11</v>
-      </c>
-      <c r="D114">
-        <v>60</v>
-      </c>
-      <c r="E114" t="b">
-        <v>0</v>
-      </c>
-      <c r="F114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>132</v>
-      </c>
-      <c r="B115" t="s">
-        <v>134</v>
-      </c>
-      <c r="C115" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115">
-        <v>160</v>
-      </c>
-      <c r="E115" t="b">
-        <v>0</v>
-      </c>
-      <c r="F115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>132</v>
-      </c>
-      <c r="B116" t="s">
-        <v>136</v>
-      </c>
-      <c r="C116" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116">
-        <v>70</v>
-      </c>
-      <c r="E116" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>132</v>
-      </c>
-      <c r="B117" t="s">
-        <v>138</v>
-      </c>
-      <c r="C117" t="s">
-        <v>11</v>
-      </c>
-      <c r="D117">
-        <v>75</v>
-      </c>
       <c r="E117" t="b">
         <v>0</v>
       </c>
@@ -3292,139 +3367,139 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>132</v>
       </c>
       <c r="B118" t="s">
+        <v>133</v>
+      </c>
+      <c r="C118" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118">
+        <v>60</v>
+      </c>
+      <c r="E118" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>132</v>
+      </c>
+      <c r="B119" t="s">
+        <v>134</v>
+      </c>
+      <c r="C119" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119">
+        <v>160</v>
+      </c>
+      <c r="E119" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>132</v>
+      </c>
+      <c r="B120" t="s">
+        <v>136</v>
+      </c>
+      <c r="C120" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120">
+        <v>70</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>132</v>
+      </c>
+      <c r="B121" t="s">
+        <v>138</v>
+      </c>
+      <c r="C121" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121">
+        <v>75</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>132</v>
+      </c>
+      <c r="B122" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" t="s">
+        <v>17</v>
+      </c>
+      <c r="D122">
+        <v>170</v>
+      </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>132</v>
+      </c>
+      <c r="B123" t="s">
+        <v>137</v>
+      </c>
+      <c r="C123" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123">
+        <v>145</v>
+      </c>
+      <c r="E123" t="b">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>132</v>
+      </c>
+      <c r="B124" t="s">
         <v>139</v>
       </c>
-      <c r="C118" t="s">
-        <v>13</v>
-      </c>
-      <c r="D118">
+      <c r="C124" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124">
         <v>9</v>
       </c>
-      <c r="E118" t="b">
-        <v>0</v>
-      </c>
-      <c r="F118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>140</v>
-      </c>
-      <c r="B119" t="s">
-        <v>148</v>
-      </c>
-      <c r="C119" t="s">
-        <v>17</v>
-      </c>
-      <c r="D119">
-        <v>75</v>
-      </c>
-      <c r="E119" t="b">
-        <v>0</v>
-      </c>
-      <c r="F119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>140</v>
-      </c>
-      <c r="B120" t="s">
-        <v>142</v>
-      </c>
-      <c r="C120" t="s">
-        <v>7</v>
-      </c>
-      <c r="D120">
-        <v>100</v>
-      </c>
-      <c r="E120" t="b">
-        <v>0</v>
-      </c>
-      <c r="F120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>140</v>
-      </c>
-      <c r="B121" t="s">
-        <v>143</v>
-      </c>
-      <c r="C121" t="s">
-        <v>11</v>
-      </c>
-      <c r="D121">
-        <v>55</v>
-      </c>
-      <c r="E121" t="b">
-        <v>0</v>
-      </c>
-      <c r="F121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>140</v>
-      </c>
-      <c r="B122" t="s">
-        <v>144</v>
-      </c>
-      <c r="C122" t="s">
-        <v>11</v>
-      </c>
-      <c r="D122">
-        <v>55</v>
-      </c>
-      <c r="E122" t="b">
-        <v>0</v>
-      </c>
-      <c r="F122">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>140</v>
-      </c>
-      <c r="B123" t="s">
-        <v>160</v>
-      </c>
-      <c r="C123" t="s">
-        <v>24</v>
-      </c>
-      <c r="D123">
-        <v>40</v>
-      </c>
-      <c r="E123" t="b">
-        <v>0</v>
-      </c>
-      <c r="F123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
-        <v>140</v>
-      </c>
-      <c r="B124" t="s">
-        <v>141</v>
-      </c>
-      <c r="C124" t="s">
-        <v>24</v>
-      </c>
-      <c r="D124">
-        <v>75</v>
-      </c>
       <c r="E124" t="b">
         <v>0</v>
       </c>
@@ -3432,18 +3507,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>140</v>
       </c>
       <c r="B125" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C125" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D125">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="E125" t="b">
         <v>0</v>
@@ -3452,18 +3527,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>140</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C126" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D126">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="E126" t="b">
         <v>0</v>
@@ -3472,18 +3547,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>140</v>
       </c>
       <c r="B127" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="C127" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D127">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="E127" t="b">
         <v>0</v>
@@ -3492,310 +3567,810 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>140</v>
       </c>
       <c r="B128" t="s">
+        <v>170</v>
+      </c>
+      <c r="C128" t="s">
+        <v>11</v>
+      </c>
+      <c r="D128">
+        <v>75</v>
+      </c>
+      <c r="E128" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>140</v>
+      </c>
+      <c r="B129" t="s">
+        <v>171</v>
+      </c>
+      <c r="C129" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129">
+        <v>65</v>
+      </c>
+      <c r="E129" t="b">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>140</v>
+      </c>
+      <c r="B130" t="s">
+        <v>173</v>
+      </c>
+      <c r="C130" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130">
+        <v>75</v>
+      </c>
+      <c r="E130" t="b">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>140</v>
+      </c>
+      <c r="B131" t="s">
+        <v>177</v>
+      </c>
+      <c r="C131" t="s">
+        <v>11</v>
+      </c>
+      <c r="D131">
+        <v>60</v>
+      </c>
+      <c r="E131" t="b">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>140</v>
+      </c>
+      <c r="B132" t="s">
+        <v>148</v>
+      </c>
+      <c r="C132" t="s">
+        <v>17</v>
+      </c>
+      <c r="D132">
+        <v>75</v>
+      </c>
+      <c r="E132" t="b">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>140</v>
+      </c>
+      <c r="B133" t="s">
+        <v>179</v>
+      </c>
+      <c r="C133" t="s">
+        <v>17</v>
+      </c>
+      <c r="D133">
+        <v>165</v>
+      </c>
+      <c r="E133" t="b">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>140</v>
+      </c>
+      <c r="B134" t="s">
+        <v>142</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134">
+        <v>100</v>
+      </c>
+      <c r="E134" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>140</v>
+      </c>
+      <c r="B135" t="s">
+        <v>172</v>
+      </c>
+      <c r="C135" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135">
+        <v>115</v>
+      </c>
+      <c r="E135" t="b">
+        <v>0</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>140</v>
+      </c>
+      <c r="B136" t="s">
+        <v>191</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136">
+        <v>80</v>
+      </c>
+      <c r="E136" t="b">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>140</v>
+      </c>
+      <c r="B137" t="s">
+        <v>145</v>
+      </c>
+      <c r="C137" t="s">
+        <v>49</v>
+      </c>
+      <c r="D137">
+        <v>25</v>
+      </c>
+      <c r="E137" t="b">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>140</v>
+      </c>
+      <c r="B138" t="s">
+        <v>167</v>
+      </c>
+      <c r="C138" t="s">
+        <v>49</v>
+      </c>
+      <c r="D138">
+        <v>65</v>
+      </c>
+      <c r="E138" t="b">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>140</v>
+      </c>
+      <c r="B139" t="s">
+        <v>178</v>
+      </c>
+      <c r="C139" t="s">
+        <v>49</v>
+      </c>
+      <c r="D139">
+        <v>30</v>
+      </c>
+      <c r="E139" t="b">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140" t="s">
+        <v>160</v>
+      </c>
+      <c r="C140" t="s">
+        <v>24</v>
+      </c>
+      <c r="D140">
+        <v>40</v>
+      </c>
+      <c r="E140" t="b">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>140</v>
+      </c>
+      <c r="B141" t="s">
+        <v>141</v>
+      </c>
+      <c r="C141" t="s">
+        <v>24</v>
+      </c>
+      <c r="D141">
+        <v>75</v>
+      </c>
+      <c r="E141" t="b">
+        <v>0</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>140</v>
+      </c>
+      <c r="B142" t="s">
+        <v>182</v>
+      </c>
+      <c r="C142" t="s">
+        <v>24</v>
+      </c>
+      <c r="D142">
+        <v>50</v>
+      </c>
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>140</v>
+      </c>
+      <c r="B143" t="s">
+        <v>146</v>
+      </c>
+      <c r="C143" t="s">
+        <v>13</v>
+      </c>
+      <c r="D143">
+        <v>14</v>
+      </c>
+      <c r="E143" t="b">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>140</v>
+      </c>
+      <c r="B144" t="s">
+        <v>147</v>
+      </c>
+      <c r="C144" t="s">
+        <v>13</v>
+      </c>
+      <c r="D144">
+        <v>10</v>
+      </c>
+      <c r="E144" t="b">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>140</v>
+      </c>
+      <c r="B145" t="s">
         <v>149</v>
       </c>
-      <c r="C128" t="s">
-        <v>13</v>
-      </c>
-      <c r="D128">
+      <c r="C145" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145">
         <v>6</v>
       </c>
-      <c r="E128" t="b">
-        <v>0</v>
-      </c>
-      <c r="F128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+      <c r="E145" t="b">
+        <v>0</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>140</v>
+      </c>
+      <c r="B146" t="s">
+        <v>186</v>
+      </c>
+      <c r="C146" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146">
+        <v>8</v>
+      </c>
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>140</v>
+      </c>
+      <c r="B147" t="s">
+        <v>188</v>
+      </c>
+      <c r="C147" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147">
+        <v>20</v>
+      </c>
+      <c r="E147" t="b">
+        <v>0</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>150</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B148" t="s">
+        <v>152</v>
+      </c>
+      <c r="C148" t="s">
+        <v>11</v>
+      </c>
+      <c r="D148">
+        <v>50</v>
+      </c>
+      <c r="E148" t="b">
+        <v>0</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>150</v>
+      </c>
+      <c r="B149" t="s">
+        <v>153</v>
+      </c>
+      <c r="C149" t="s">
+        <v>11</v>
+      </c>
+      <c r="D149">
+        <v>60</v>
+      </c>
+      <c r="E149" t="b">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150" t="s">
+        <v>156</v>
+      </c>
+      <c r="C150" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150">
+        <v>80</v>
+      </c>
+      <c r="E150" t="b">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+      <c r="B151" t="s">
+        <v>159</v>
+      </c>
+      <c r="C151" t="s">
+        <v>17</v>
+      </c>
+      <c r="D151">
+        <v>100</v>
+      </c>
+      <c r="E151" t="b">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>150</v>
+      </c>
+      <c r="B152" t="s">
         <v>166</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C152" t="s">
         <v>7</v>
       </c>
-      <c r="D129">
+      <c r="D152">
         <v>130</v>
       </c>
-      <c r="E129" t="b">
-        <v>0</v>
-      </c>
-      <c r="F129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+      <c r="E152" t="b">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>150</v>
       </c>
-      <c r="B130" t="s">
-        <v>159</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="B153" t="s">
+        <v>151</v>
+      </c>
+      <c r="C153" t="s">
+        <v>13</v>
+      </c>
+      <c r="D153">
+        <v>9</v>
+      </c>
+      <c r="E153" t="b">
+        <v>0</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>150</v>
+      </c>
+      <c r="B154" t="s">
+        <v>154</v>
+      </c>
+      <c r="C154" t="s">
+        <v>13</v>
+      </c>
+      <c r="D154">
+        <v>11</v>
+      </c>
+      <c r="E154" t="b">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>150</v>
+      </c>
+      <c r="B155" t="s">
+        <v>155</v>
+      </c>
+      <c r="C155" t="s">
+        <v>13</v>
+      </c>
+      <c r="D155">
+        <v>6</v>
+      </c>
+      <c r="E155" t="b">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" t="s">
+        <v>157</v>
+      </c>
+      <c r="C156" t="s">
+        <v>13</v>
+      </c>
+      <c r="D156">
+        <v>8</v>
+      </c>
+      <c r="E156" t="b">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>150</v>
+      </c>
+      <c r="B157" t="s">
+        <v>161</v>
+      </c>
+      <c r="C157" t="s">
+        <v>13</v>
+      </c>
+      <c r="D157">
+        <v>9</v>
+      </c>
+      <c r="E157" t="b">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>150</v>
+      </c>
+      <c r="B158" t="s">
+        <v>158</v>
+      </c>
+      <c r="C158" t="s">
+        <v>13</v>
+      </c>
+      <c r="D158">
+        <v>13</v>
+      </c>
+      <c r="E158" t="b">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>3</v>
+      </c>
+      <c r="B159" t="s">
+        <v>174</v>
+      </c>
+      <c r="C159" t="s">
+        <v>11</v>
+      </c>
+      <c r="D159">
+        <v>60</v>
+      </c>
+      <c r="E159" t="b">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>3</v>
+      </c>
+      <c r="B160" t="s">
+        <v>187</v>
+      </c>
+      <c r="C160" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160">
+        <v>40</v>
+      </c>
+      <c r="E160" t="b">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>3</v>
+      </c>
+      <c r="B161" t="s">
+        <v>175</v>
+      </c>
+      <c r="C161" t="s">
         <v>17</v>
       </c>
-      <c r="D130">
+      <c r="D161">
+        <v>170</v>
+      </c>
+      <c r="E161" t="b">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162" t="s">
+        <v>7</v>
+      </c>
+      <c r="D162">
+        <v>160</v>
+      </c>
+      <c r="E162" t="b">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163">
         <v>100</v>
       </c>
-      <c r="E130" t="b">
-        <v>0</v>
-      </c>
-      <c r="F130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>150</v>
-      </c>
-      <c r="B131" t="s">
-        <v>152</v>
-      </c>
-      <c r="C131" t="s">
-        <v>11</v>
-      </c>
-      <c r="D131">
-        <v>50</v>
-      </c>
-      <c r="E131" t="b">
-        <v>0</v>
-      </c>
-      <c r="F131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>150</v>
-      </c>
-      <c r="B132" t="s">
-        <v>153</v>
-      </c>
-      <c r="C132" t="s">
-        <v>11</v>
-      </c>
-      <c r="D132">
-        <v>60</v>
-      </c>
-      <c r="E132" t="b">
-        <v>0</v>
-      </c>
-      <c r="F132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>150</v>
-      </c>
-      <c r="B133" t="s">
-        <v>156</v>
-      </c>
-      <c r="C133" t="s">
-        <v>11</v>
-      </c>
-      <c r="D133">
-        <v>80</v>
-      </c>
-      <c r="E133" t="b">
-        <v>0</v>
-      </c>
-      <c r="F133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>150</v>
-      </c>
-      <c r="B134" t="s">
-        <v>151</v>
-      </c>
-      <c r="C134" t="s">
-        <v>13</v>
-      </c>
-      <c r="D134">
-        <v>9</v>
-      </c>
-      <c r="E134" t="b">
-        <v>0</v>
-      </c>
-      <c r="F134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>150</v>
-      </c>
-      <c r="B135" t="s">
-        <v>154</v>
-      </c>
-      <c r="C135" t="s">
-        <v>13</v>
-      </c>
-      <c r="D135">
-        <v>11</v>
-      </c>
-      <c r="E135" t="b">
-        <v>0</v>
-      </c>
-      <c r="F135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>150</v>
-      </c>
-      <c r="B136" t="s">
-        <v>155</v>
-      </c>
-      <c r="C136" t="s">
-        <v>13</v>
-      </c>
-      <c r="D136">
+      <c r="E163" t="b">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>3</v>
+      </c>
+      <c r="B164" t="s">
         <v>6</v>
       </c>
-      <c r="E136" t="b">
-        <v>0</v>
-      </c>
-      <c r="F136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>150</v>
-      </c>
-      <c r="B137" t="s">
-        <v>157</v>
-      </c>
-      <c r="C137" t="s">
-        <v>13</v>
-      </c>
-      <c r="D137">
-        <v>8</v>
-      </c>
-      <c r="E137" t="b">
-        <v>0</v>
-      </c>
-      <c r="F137">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>150</v>
-      </c>
-      <c r="B138" t="s">
-        <v>161</v>
-      </c>
-      <c r="C138" t="s">
-        <v>13</v>
-      </c>
-      <c r="D138">
-        <v>9</v>
-      </c>
-      <c r="E138" t="b">
-        <v>0</v>
-      </c>
-      <c r="F138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>150</v>
-      </c>
-      <c r="B139" t="s">
-        <v>158</v>
-      </c>
-      <c r="C139" t="s">
-        <v>13</v>
-      </c>
-      <c r="D139">
-        <v>13</v>
-      </c>
-      <c r="E139" t="b">
-        <v>0</v>
-      </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+      <c r="C164" t="s">
+        <v>7</v>
+      </c>
+      <c r="D164">
+        <v>100</v>
+      </c>
+      <c r="E164" t="b">
+        <v>0</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>3</v>
       </c>
-      <c r="B140" t="s">
-        <v>4</v>
-      </c>
-      <c r="C140" t="s">
+      <c r="B165" t="s">
+        <v>168</v>
+      </c>
+      <c r="C165" t="s">
         <v>7</v>
       </c>
-      <c r="D140">
-        <v>160</v>
-      </c>
-      <c r="E140" t="b">
-        <v>0</v>
-      </c>
-      <c r="F140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
+      <c r="D165">
+        <v>95</v>
+      </c>
+      <c r="E165" t="b">
+        <v>0</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>3</v>
       </c>
-      <c r="B141" t="s">
-        <v>5</v>
-      </c>
-      <c r="C141" t="s">
-        <v>7</v>
-      </c>
-      <c r="D141">
-        <v>100</v>
-      </c>
-      <c r="E141" t="b">
-        <v>0</v>
-      </c>
-      <c r="F141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+      <c r="B166" t="s">
+        <v>183</v>
+      </c>
+      <c r="C166" t="s">
+        <v>24</v>
+      </c>
+      <c r="D166">
+        <v>10</v>
+      </c>
+      <c r="E166" t="b">
+        <v>0</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>3</v>
       </c>
-      <c r="B142" t="s">
-        <v>6</v>
-      </c>
-      <c r="C142" t="s">
-        <v>7</v>
-      </c>
-      <c r="D142">
-        <v>100</v>
-      </c>
-      <c r="E142" t="b">
-        <v>0</v>
-      </c>
-      <c r="F142">
+      <c r="B167" t="s">
+        <v>185</v>
+      </c>
+      <c r="C167" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167">
+        <v>10</v>
+      </c>
+      <c r="E167" t="b">
+        <v>0</v>
+      </c>
+      <c r="F167">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D142">
-    <sortCondition ref="A2:A142"/>
-    <sortCondition ref="C2:C142"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F167">
+    <sortCondition ref="A2:A167"/>
+    <sortCondition ref="C2:C167"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New batch of profiles, and various backend improvements
</commit_message>
<xml_diff>
--- a/src/mesbg_models.xlsx
+++ b/src/mesbg_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65AE9B9-E1C2-46C7-81BC-EE75A6F8BFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB744FB-4B34-4349-ABF1-7D9061751E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="213">
   <si>
     <t>faction</t>
   </si>
@@ -615,6 +615,69 @@
   </si>
   <si>
     <t>Theodred</t>
+  </si>
+  <si>
+    <t>Bill the Pony</t>
+  </si>
+  <si>
+    <t>Smeagol</t>
+  </si>
+  <si>
+    <t>Ringwraith</t>
+  </si>
+  <si>
+    <t>Shelob</t>
+  </si>
+  <si>
+    <t>Orc Taskmaster</t>
+  </si>
+  <si>
+    <t>Black Guard Drummer</t>
+  </si>
+  <si>
+    <t>Gothmog's Enforcer</t>
+  </si>
+  <si>
+    <t>Zagdush</t>
+  </si>
+  <si>
+    <t>Goroth</t>
+  </si>
+  <si>
+    <t>Muzgur</t>
+  </si>
+  <si>
+    <t>Razgush</t>
+  </si>
+  <si>
+    <t>Orc Tracker</t>
+  </si>
+  <si>
+    <t>Morgul Stalker</t>
+  </si>
+  <si>
+    <t>Mordor War Catapult</t>
+  </si>
+  <si>
+    <t>Mordor Siege Bow</t>
+  </si>
+  <si>
+    <t>Great Beast of Gorgoroth</t>
+  </si>
+  <si>
+    <t>Uruk-Hai Captain</t>
+  </si>
+  <si>
+    <t>Snaga</t>
+  </si>
+  <si>
+    <t>Feral Uruk-Hai</t>
+  </si>
+  <si>
+    <t>Isengard Assault Ballista</t>
+  </si>
+  <si>
+    <t>Uruk-Hai Demolition Team</t>
   </si>
 </sst>
 </file>
@@ -1010,17 +1073,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G159" sqref="G159"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H161" sqref="H161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1092,13 +1155,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -1112,13 +1175,13 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5">
-        <v>24</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -1132,13 +1195,13 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -1172,13 +1235,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8">
-        <v>140</v>
+        <v>75</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1192,13 +1255,13 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1212,13 +1275,13 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10">
-        <v>110</v>
+        <v>160</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1232,13 +1295,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="D11">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1292,13 +1355,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1312,13 +1375,13 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1332,13 +1395,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1352,13 +1415,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1372,13 +1435,13 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1412,13 +1475,13 @@
         <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1432,13 +1495,13 @@
         <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
       <c r="D21">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1532,13 +1595,13 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
       </c>
       <c r="D26">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1572,13 +1635,13 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
       </c>
       <c r="D28">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1592,13 +1655,13 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
       </c>
       <c r="D29">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1652,13 +1715,13 @@
         <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1672,13 +1735,13 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1692,13 +1755,13 @@
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
       </c>
       <c r="D34">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1712,13 +1775,13 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>208</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1732,13 +1795,13 @@
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="D36">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1752,13 +1815,13 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D37">
-        <v>180</v>
+        <v>50</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1772,13 +1835,13 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1792,13 +1855,13 @@
         <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D39">
-        <v>25</v>
+        <v>180</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1812,13 +1875,13 @@
         <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="D40">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1832,13 +1895,13 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D41">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1852,13 +1915,13 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D42">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1872,13 +1935,13 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D43">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1892,19 +1955,19 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>212</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D44">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1912,33 +1975,33 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>211</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D45">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D46">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1949,16 +2012,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D47">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1969,16 +2032,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>210</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D48">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1989,16 +2052,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D49">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -2009,16 +2072,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D50">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -2032,13 +2095,13 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D51">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2052,13 +2115,13 @@
         <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D52">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -2072,13 +2135,13 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D53">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -2092,13 +2155,13 @@
         <v>63</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D54">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -2112,13 +2175,13 @@
         <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D55">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -2132,16 +2195,16 @@
         <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D56">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="E56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -2152,13 +2215,13 @@
         <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D57">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
@@ -2169,19 +2232,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D58">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -2189,16 +2252,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D59">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -2209,16 +2272,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D60">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -2229,16 +2292,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D61">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -2249,16 +2312,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D62">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -2272,13 +2335,13 @@
         <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
         <v>11</v>
       </c>
       <c r="D63">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -2292,13 +2355,13 @@
         <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C64" t="s">
         <v>11</v>
       </c>
       <c r="D64">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -2312,13 +2375,13 @@
         <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C65" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D65">
-        <v>225</v>
+        <v>60</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -2332,13 +2395,13 @@
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D66">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -2352,13 +2415,13 @@
         <v>76</v>
       </c>
       <c r="B67" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D67">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -2372,13 +2435,13 @@
         <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D68">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
@@ -2392,13 +2455,13 @@
         <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D69">
-        <v>220</v>
+        <v>50</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -2412,13 +2475,13 @@
         <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D70">
-        <v>80</v>
+        <v>225</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -2432,13 +2495,13 @@
         <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C71" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="D71">
-        <v>25</v>
+        <v>220</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
@@ -2452,13 +2515,13 @@
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C72" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D72">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
@@ -2472,13 +2535,13 @@
         <v>76</v>
       </c>
       <c r="B73" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73">
         <v>80</v>
-      </c>
-      <c r="C73" t="s">
-        <v>24</v>
-      </c>
-      <c r="D73">
-        <v>30</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
@@ -2492,13 +2555,13 @@
         <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C74" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D74">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
@@ -2512,10 +2575,10 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C75" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D75">
         <v>35</v>
@@ -2532,19 +2595,19 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C76" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D76">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2552,19 +2615,19 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>176</v>
+        <v>77</v>
       </c>
       <c r="C77" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D77">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="E77" t="b">
         <v>0</v>
       </c>
       <c r="F77">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2572,13 +2635,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C78" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D78">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
@@ -2592,13 +2655,13 @@
         <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D79">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
@@ -2612,13 +2675,13 @@
         <v>76</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C80" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D80">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
@@ -2632,19 +2695,19 @@
         <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>96</v>
+        <v>176</v>
       </c>
       <c r="C81" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D81">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="E81" t="b">
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2652,19 +2715,19 @@
         <v>76</v>
       </c>
       <c r="B82" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C82" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D82">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="E82" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2672,13 +2735,13 @@
         <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C83" t="s">
         <v>13</v>
       </c>
       <c r="D83">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
@@ -2689,16 +2752,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B84" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C84" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D84">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E84" t="b">
         <v>0</v>
@@ -2709,16 +2772,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D85">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E85" t="b">
         <v>0</v>
@@ -2729,16 +2792,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C86" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D86">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="E86" t="b">
         <v>0</v>
@@ -2749,19 +2812,19 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B87" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C87" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D87">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="E87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87">
         <v>0</v>
@@ -2769,16 +2832,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C88" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D88">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="E88" t="b">
         <v>0</v>
@@ -2789,16 +2852,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B89" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D89">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="E89" t="b">
         <v>0</v>
@@ -2812,19 +2875,19 @@
         <v>102</v>
       </c>
       <c r="B90" t="s">
-        <v>110</v>
+        <v>207</v>
       </c>
       <c r="C90" t="s">
         <v>11</v>
       </c>
       <c r="D90">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="E90" t="b">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2832,13 +2895,13 @@
         <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
       </c>
       <c r="D91">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="E91" t="b">
         <v>0</v>
@@ -2852,13 +2915,13 @@
         <v>102</v>
       </c>
       <c r="B92" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C92" t="s">
         <v>11</v>
       </c>
       <c r="D92">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="E92" t="b">
         <v>0</v>
@@ -2872,13 +2935,13 @@
         <v>102</v>
       </c>
       <c r="B93" t="s">
-        <v>116</v>
+        <v>200</v>
       </c>
       <c r="C93" t="s">
         <v>11</v>
       </c>
       <c r="D93">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E93" t="b">
         <v>0</v>
@@ -2892,13 +2955,13 @@
         <v>102</v>
       </c>
       <c r="B94" t="s">
-        <v>119</v>
+        <v>201</v>
       </c>
       <c r="C94" t="s">
         <v>11</v>
       </c>
       <c r="D94">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E94" t="b">
         <v>0</v>
@@ -2912,13 +2975,13 @@
         <v>102</v>
       </c>
       <c r="B95" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C95" t="s">
         <v>11</v>
       </c>
       <c r="D95">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -2932,13 +2995,13 @@
         <v>102</v>
       </c>
       <c r="B96" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C96" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D96">
-        <v>400</v>
+        <v>65</v>
       </c>
       <c r="E96" t="b">
         <v>0</v>
@@ -2952,13 +3015,13 @@
         <v>102</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="C97" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D97">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E97" t="b">
         <v>0</v>
@@ -2972,13 +3035,13 @@
         <v>102</v>
       </c>
       <c r="B98" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C98" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D98">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="E98" t="b">
         <v>0</v>
@@ -2992,13 +3055,13 @@
         <v>102</v>
       </c>
       <c r="B99" t="s">
-        <v>111</v>
+        <v>198</v>
       </c>
       <c r="C99" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D99">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
@@ -3012,13 +3075,13 @@
         <v>102</v>
       </c>
       <c r="B100" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="C100" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D100">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="E100" t="b">
         <v>0</v>
@@ -3032,13 +3095,13 @@
         <v>102</v>
       </c>
       <c r="B101" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="C101" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D101">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E101" t="b">
         <v>0</v>
@@ -3052,13 +3115,13 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C102" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D102">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
@@ -3072,13 +3135,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>194</v>
       </c>
       <c r="C103" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D103">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="E103" t="b">
         <v>0</v>
@@ -3092,13 +3155,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C104" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D104">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -3112,13 +3175,13 @@
         <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>184</v>
+        <v>112</v>
       </c>
       <c r="C105" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D105">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -3132,13 +3195,13 @@
         <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C106" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D106">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="E106" t="b">
         <v>0</v>
@@ -3152,13 +3215,13 @@
         <v>102</v>
       </c>
       <c r="B107" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D107">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="E107" t="b">
         <v>0</v>
@@ -3172,13 +3235,13 @@
         <v>102</v>
       </c>
       <c r="B108" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C108" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D108">
-        <v>30</v>
+        <v>400</v>
       </c>
       <c r="E108" t="b">
         <v>0</v>
@@ -3192,13 +3255,13 @@
         <v>102</v>
       </c>
       <c r="B109" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="C109" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D109">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
@@ -3212,13 +3275,13 @@
         <v>102</v>
       </c>
       <c r="B110" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D110">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="E110" t="b">
         <v>0</v>
@@ -3232,13 +3295,13 @@
         <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C111" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D111">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
@@ -3252,13 +3315,13 @@
         <v>102</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C112" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D112">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E112" t="b">
         <v>0</v>
@@ -3272,13 +3335,13 @@
         <v>102</v>
       </c>
       <c r="B113" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C113" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D113">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
@@ -3292,13 +3355,13 @@
         <v>102</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C114" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D114">
-        <v>18</v>
+        <v>120</v>
       </c>
       <c r="E114" t="b">
         <v>0</v>
@@ -3312,13 +3375,13 @@
         <v>102</v>
       </c>
       <c r="B115" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C115" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D115">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E115" t="b">
         <v>0</v>
@@ -3332,13 +3395,13 @@
         <v>102</v>
       </c>
       <c r="B116" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C116" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D116">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="E116" t="b">
         <v>0</v>
@@ -3352,13 +3415,13 @@
         <v>102</v>
       </c>
       <c r="B117" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="C117" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D117">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="E117" t="b">
         <v>0</v>
@@ -3369,16 +3432,16 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B118" t="s">
-        <v>133</v>
+        <v>190</v>
       </c>
       <c r="C118" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D118">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="E118" t="b">
         <v>0</v>
@@ -3389,16 +3452,16 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B119" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="C119" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D119">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="E119" t="b">
         <v>0</v>
@@ -3409,13 +3472,13 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B120" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="C120" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D120">
         <v>70</v>
@@ -3429,16 +3492,16 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B121" t="s">
-        <v>138</v>
+        <v>195</v>
       </c>
       <c r="C121" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D121">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E121" t="b">
         <v>0</v>
@@ -3449,16 +3512,16 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B122" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="C122" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D122">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="E122" t="b">
         <v>0</v>
@@ -3469,16 +3532,16 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B123" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="C123" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D123">
-        <v>145</v>
+        <v>30</v>
       </c>
       <c r="E123" t="b">
         <v>0</v>
@@ -3489,16 +3552,16 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B124" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C124" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D124">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E124" t="b">
         <v>0</v>
@@ -3509,56 +3572,56 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B125" t="s">
-        <v>143</v>
+        <v>205</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D125">
-        <v>55</v>
+        <v>160</v>
       </c>
       <c r="E125" t="b">
         <v>0</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B126" t="s">
-        <v>144</v>
+        <v>206</v>
       </c>
       <c r="C126" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D126">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E126" t="b">
         <v>0</v>
       </c>
       <c r="F126">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B127" t="s">
-        <v>169</v>
+        <v>115</v>
       </c>
       <c r="C127" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D127">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="E127" t="b">
         <v>0</v>
@@ -3569,16 +3632,16 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B128" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="C128" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D128">
-        <v>75</v>
+        <v>18</v>
       </c>
       <c r="E128" t="b">
         <v>0</v>
@@ -3589,16 +3652,16 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B129" t="s">
-        <v>171</v>
+        <v>103</v>
       </c>
       <c r="C129" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D129">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="E129" t="b">
         <v>0</v>
@@ -3609,16 +3672,16 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B130" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="C130" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D130">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="E130" t="b">
         <v>0</v>
@@ -3629,16 +3692,16 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B131" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="C131" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D131">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="E131" t="b">
         <v>0</v>
@@ -3649,16 +3712,16 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B132" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="C132" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D132">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="E132" t="b">
         <v>0</v>
@@ -3669,16 +3732,16 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B133" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C133" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D133">
-        <v>165</v>
+        <v>8</v>
       </c>
       <c r="E133" t="b">
         <v>0</v>
@@ -3689,16 +3752,16 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B134" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C134" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134">
         <v>7</v>
-      </c>
-      <c r="D134">
-        <v>100</v>
       </c>
       <c r="E134" t="b">
         <v>0</v>
@@ -3709,16 +3772,16 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B135" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="C135" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D135">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="E135" t="b">
         <v>0</v>
@@ -3729,19 +3792,19 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="B136" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="C136" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D136">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="E136" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F136">
         <v>0</v>
@@ -3749,16 +3812,16 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C137" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D137">
-        <v>25</v>
+        <v>160</v>
       </c>
       <c r="E137" t="b">
         <v>0</v>
@@ -3769,19 +3832,19 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B138" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="C138" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D138">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F138">
         <v>0</v>
@@ -3789,16 +3852,16 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B139" t="s">
-        <v>178</v>
+        <v>136</v>
       </c>
       <c r="C139" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="D139">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="E139" t="b">
         <v>0</v>
@@ -3809,16 +3872,16 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B140" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="C140" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D140">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E140" t="b">
         <v>0</v>
@@ -3829,16 +3892,16 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B141" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C141" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D141">
-        <v>75</v>
+        <v>170</v>
       </c>
       <c r="E141" t="b">
         <v>0</v>
@@ -3849,19 +3912,19 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B142" t="s">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="C142" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D142">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="E142" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F142">
         <v>0</v>
@@ -3869,16 +3932,16 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B143" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C143" t="s">
         <v>13</v>
       </c>
       <c r="D143">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E143" t="b">
         <v>0</v>
@@ -3892,13 +3955,13 @@
         <v>140</v>
       </c>
       <c r="B144" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="C144" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D144">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="E144" t="b">
         <v>0</v>
@@ -3912,13 +3975,13 @@
         <v>140</v>
       </c>
       <c r="B145" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="C145" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D145">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="E145" t="b">
         <v>0</v>
@@ -3932,16 +3995,16 @@
         <v>140</v>
       </c>
       <c r="B146" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="C146" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D146">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="E146" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -3952,13 +4015,13 @@
         <v>140</v>
       </c>
       <c r="B147" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C147" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D147">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E147" t="b">
         <v>0</v>
@@ -3969,16 +4032,16 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B148" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C148" t="s">
         <v>11</v>
       </c>
       <c r="D148">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E148" t="b">
         <v>0</v>
@@ -3989,16 +4052,16 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B149" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C149" t="s">
         <v>11</v>
       </c>
       <c r="D149">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E149" t="b">
         <v>0</v>
@@ -4009,16 +4072,16 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B150" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="C150" t="s">
         <v>11</v>
       </c>
       <c r="D150">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="E150" t="b">
         <v>0</v>
@@ -4029,16 +4092,16 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B151" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="C151" t="s">
         <v>17</v>
       </c>
       <c r="D151">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="E151" t="b">
         <v>0</v>
@@ -4049,16 +4112,16 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B152" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="C152" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D152">
-        <v>130</v>
+        <v>75</v>
       </c>
       <c r="E152" t="b">
         <v>0</v>
@@ -4069,16 +4132,16 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B153" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="C153" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D153">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="E153" t="b">
         <v>0</v>
@@ -4089,16 +4152,16 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B154" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C154" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D154">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="E154" t="b">
         <v>0</v>
@@ -4109,16 +4172,16 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B155" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="C155" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D155">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="E155" t="b">
         <v>0</v>
@@ -4129,19 +4192,19 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B156" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C156" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D156">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="E156" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F156">
         <v>0</v>
@@ -4149,16 +4212,16 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B157" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="C157" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D157">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E157" t="b">
         <v>0</v>
@@ -4169,16 +4232,16 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B158" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C158" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D158">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E158" t="b">
         <v>0</v>
@@ -4189,16 +4252,16 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B159" t="s">
-        <v>174</v>
+        <v>141</v>
       </c>
       <c r="C159" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D159">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E159" t="b">
         <v>0</v>
@@ -4209,19 +4272,19 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B160" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C160" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D160">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E160" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F160">
         <v>0</v>
@@ -4229,16 +4292,16 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B161" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="C161" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D161">
-        <v>170</v>
+        <v>40</v>
       </c>
       <c r="E161" t="b">
         <v>0</v>
@@ -4249,16 +4312,16 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B162" t="s">
-        <v>4</v>
+        <v>188</v>
       </c>
       <c r="C162" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D162">
-        <v>160</v>
+        <v>20</v>
       </c>
       <c r="E162" t="b">
         <v>0</v>
@@ -4269,16 +4332,16 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B163" t="s">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="C163" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D163">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="E163" t="b">
         <v>0</v>
@@ -4289,16 +4352,16 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B164" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C164" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D164">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E164" t="b">
         <v>0</v>
@@ -4309,19 +4372,19 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B165" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="C165" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D165">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E165" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F165">
         <v>0</v>
@@ -4329,16 +4392,16 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>3</v>
+        <v>140</v>
       </c>
       <c r="B166" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="C166" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D166">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E166" t="b">
         <v>0</v>
@@ -4349,28 +4412,449 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
+        <v>150</v>
+      </c>
+      <c r="B167" t="s">
+        <v>156</v>
+      </c>
+      <c r="C167" t="s">
+        <v>11</v>
+      </c>
+      <c r="D167">
+        <v>80</v>
+      </c>
+      <c r="E167" t="b">
+        <v>0</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>150</v>
+      </c>
+      <c r="B168" t="s">
+        <v>153</v>
+      </c>
+      <c r="C168" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168">
+        <v>60</v>
+      </c>
+      <c r="E168" t="b">
+        <v>0</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>150</v>
+      </c>
+      <c r="B169" t="s">
+        <v>152</v>
+      </c>
+      <c r="C169" t="s">
+        <v>11</v>
+      </c>
+      <c r="D169">
+        <v>50</v>
+      </c>
+      <c r="E169" t="b">
+        <v>0</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>150</v>
+      </c>
+      <c r="B170" t="s">
+        <v>159</v>
+      </c>
+      <c r="C170" t="s">
+        <v>17</v>
+      </c>
+      <c r="D170">
+        <v>100</v>
+      </c>
+      <c r="E170" t="b">
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>150</v>
+      </c>
+      <c r="B171" t="s">
+        <v>166</v>
+      </c>
+      <c r="C171" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171">
+        <v>130</v>
+      </c>
+      <c r="E171" t="b">
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>150</v>
+      </c>
+      <c r="B172" t="s">
+        <v>158</v>
+      </c>
+      <c r="C172" t="s">
+        <v>13</v>
+      </c>
+      <c r="D172">
+        <v>13</v>
+      </c>
+      <c r="E172" t="b">
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>150</v>
+      </c>
+      <c r="B173" t="s">
+        <v>154</v>
+      </c>
+      <c r="C173" t="s">
+        <v>13</v>
+      </c>
+      <c r="D173">
+        <v>11</v>
+      </c>
+      <c r="E173" t="b">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>150</v>
+      </c>
+      <c r="B174" t="s">
+        <v>151</v>
+      </c>
+      <c r="C174" t="s">
+        <v>13</v>
+      </c>
+      <c r="D174">
+        <v>9</v>
+      </c>
+      <c r="E174" t="b">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>150</v>
+      </c>
+      <c r="B175" t="s">
+        <v>161</v>
+      </c>
+      <c r="C175" t="s">
+        <v>13</v>
+      </c>
+      <c r="D175">
+        <v>9</v>
+      </c>
+      <c r="E175" t="b">
+        <v>0</v>
+      </c>
+      <c r="F175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>150</v>
+      </c>
+      <c r="B176" t="s">
+        <v>157</v>
+      </c>
+      <c r="C176" t="s">
+        <v>13</v>
+      </c>
+      <c r="D176">
+        <v>8</v>
+      </c>
+      <c r="E176" t="b">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>150</v>
+      </c>
+      <c r="B177" t="s">
+        <v>155</v>
+      </c>
+      <c r="C177" t="s">
+        <v>13</v>
+      </c>
+      <c r="D177">
+        <v>6</v>
+      </c>
+      <c r="E177" t="b">
+        <v>0</v>
+      </c>
+      <c r="F177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>3</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B178" t="s">
+        <v>174</v>
+      </c>
+      <c r="C178" t="s">
+        <v>11</v>
+      </c>
+      <c r="D178">
+        <v>60</v>
+      </c>
+      <c r="E178" t="b">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>3</v>
+      </c>
+      <c r="B179" t="s">
+        <v>187</v>
+      </c>
+      <c r="C179" t="s">
+        <v>11</v>
+      </c>
+      <c r="D179">
+        <v>40</v>
+      </c>
+      <c r="E179" t="b">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" t="s">
+        <v>175</v>
+      </c>
+      <c r="C180" t="s">
+        <v>17</v>
+      </c>
+      <c r="D180">
+        <v>170</v>
+      </c>
+      <c r="E180" t="b">
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>3</v>
+      </c>
+      <c r="B181" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181" t="s">
+        <v>7</v>
+      </c>
+      <c r="D181">
+        <v>160</v>
+      </c>
+      <c r="E181" t="b">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182" t="s">
+        <v>5</v>
+      </c>
+      <c r="C182" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182">
+        <v>100</v>
+      </c>
+      <c r="E182" t="b">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>3</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183" t="s">
+        <v>7</v>
+      </c>
+      <c r="D183">
+        <v>100</v>
+      </c>
+      <c r="E183" t="b">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>168</v>
+      </c>
+      <c r="C184" t="s">
+        <v>7</v>
+      </c>
+      <c r="D184">
+        <v>95</v>
+      </c>
+      <c r="E184" t="b">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>3</v>
+      </c>
+      <c r="B185" t="s">
+        <v>193</v>
+      </c>
+      <c r="C185" t="s">
+        <v>49</v>
+      </c>
+      <c r="D185">
+        <v>30</v>
+      </c>
+      <c r="E185" t="b">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186" t="s">
+        <v>192</v>
+      </c>
+      <c r="C186" t="s">
+        <v>49</v>
+      </c>
+      <c r="D186">
+        <v>25</v>
+      </c>
+      <c r="E186" t="b">
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>3</v>
+      </c>
+      <c r="B187" t="s">
+        <v>183</v>
+      </c>
+      <c r="C187" t="s">
+        <v>24</v>
+      </c>
+      <c r="D187">
+        <v>10</v>
+      </c>
+      <c r="E187" t="b">
+        <v>0</v>
+      </c>
+      <c r="F187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" t="s">
         <v>185</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C188" t="s">
         <v>24</v>
       </c>
-      <c r="D167">
+      <c r="D188">
         <v>10</v>
       </c>
-      <c r="E167" t="b">
-        <v>0</v>
-      </c>
-      <c r="F167">
+      <c r="E188" t="b">
+        <v>0</v>
+      </c>
+      <c r="F188">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F167">
-    <sortCondition ref="A2:A167"/>
-    <sortCondition ref="C2:C167"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F188">
+    <sortCondition ref="A2:A188"/>
+    <sortCondition ref="C2:C188"/>
+    <sortCondition descending="1" ref="D2:D188"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Demolition team is now a warrior, rather than siege engine
</commit_message>
<xml_diff>
--- a/src/mesbg_models.xlsx
+++ b/src/mesbg_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA503C7-6E72-479D-97CB-5A885AA9AB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA2F3C9-58F8-4F29-8574-3679E15F765B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -1198,24 +1198,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
   <dimension ref="A1:H268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D249" sqref="D249"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>206</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>208</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>208</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>208</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>208</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>208</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>208</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>208</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>208</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>208</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>208</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>208</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>208</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>208</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>208</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>208</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>208</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>208</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>207</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>208</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>208</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>208</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>208</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>208</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>208</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>208</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>208</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>208</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>208</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>208</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>208</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>208</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>208</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>208</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>208</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>208</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>208</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>205</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F42">
         <v>80</v>
@@ -2307,7 +2307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>208</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>208</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>208</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>208</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>208</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>208</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>208</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>208</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>208</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>208</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>208</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>208</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>208</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>207</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>207</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>207</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>207</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>207</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>207</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>207</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>207</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>207</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>207</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>207</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>207</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>207</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>207</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>207</v>
       </c>
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>207</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>207</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>207</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>207</v>
       </c>
@@ -3139,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>207</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>207</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>207</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>207</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>207</v>
       </c>
@@ -3269,7 +3269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>207</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>207</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>207</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>207</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>207</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>207</v>
       </c>
@@ -3425,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>207</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>207</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>207</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>207</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>207</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>207</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>207</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>207</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>207</v>
       </c>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>208</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>208</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>208</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>208</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>208</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>208</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>208</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>208</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>208</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>208</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>208</v>
       </c>
@@ -3945,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>208</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>208</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>208</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>208</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>208</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>208</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>208</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>208</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>208</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>208</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>208</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>208</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>208</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>208</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>208</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>208</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>208</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>208</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>208</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>208</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>208</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>208</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>208</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>208</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>208</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>208</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>208</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>208</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>208</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>208</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>208</v>
       </c>
@@ -4751,7 +4751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>208</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>208</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>208</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>208</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>207</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>207</v>
       </c>
@@ -4907,7 +4907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>207</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>207</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>207</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>207</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>207</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>207</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>207</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>207</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>207</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>207</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>207</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>207</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>207</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>207</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>207</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>207</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>207</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>207</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>207</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>207</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>207</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>207</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>207</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>207</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>207</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>207</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>207</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>207</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>207</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>207</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>207</v>
       </c>
@@ -5713,7 +5713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>207</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>207</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>207</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>207</v>
       </c>
@@ -5817,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>207</v>
       </c>
@@ -5843,7 +5843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>207</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>207</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>207</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>208</v>
       </c>
@@ -5947,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>208</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>208</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>208</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>208</v>
       </c>
@@ -6051,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>208</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>208</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>208</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>208</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>208</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>208</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>208</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>207</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>207</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>207</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>207</v>
       </c>
@@ -6337,7 +6337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>207</v>
       </c>
@@ -6363,7 +6363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>207</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>207</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>207</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -6467,7 +6467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>207</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>207</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>207</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>207</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>207</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>207</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>207</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>207</v>
       </c>
@@ -6675,7 +6675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>207</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>207</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>207</v>
       </c>
@@ -6753,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>207</v>
       </c>
@@ -6779,7 +6779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>215</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>215</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>215</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>215</v>
       </c>
@@ -6883,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>215</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>215</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>215</v>
       </c>
@@ -6961,7 +6961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>215</v>
       </c>
@@ -6987,7 +6987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>215</v>
       </c>
@@ -7013,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>215</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>207</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>207</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>207</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>207</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>207</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>207</v>
       </c>
@@ -7195,7 +7195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>207</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>207</v>
       </c>
@@ -7247,7 +7247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>207</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>207</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>207</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>207</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>207</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>207</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>207</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>207</v>
       </c>
@@ -7455,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>207</v>
       </c>
@@ -7481,7 +7481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>207</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>207</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>207</v>
       </c>
@@ -7559,7 +7559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>207</v>
       </c>
@@ -7585,7 +7585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>207</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>207</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>207</v>
       </c>
@@ -7663,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>207</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>214</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>214</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>214</v>
       </c>
@@ -7767,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>214</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>214</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>214</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>214</v>
       </c>
@@ -7871,7 +7871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>208</v>
       </c>
@@ -7897,7 +7897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>208</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>208</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>208</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>208</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>208</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>208</v>
       </c>
@@ -8053,7 +8053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>208</v>
       </c>
@@ -8079,7 +8079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>208</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>208</v>
       </c>
@@ -8131,7 +8131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>208</v>
       </c>
@@ -8157,7 +8157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>208</v>
       </c>

</xml_diff>